<commit_message>
hotfix: Bear Necessities somehow having one missing value?
</commit_message>
<xml_diff>
--- a/data/labels/song_theme_label_database.xlsx
+++ b/data/labels/song_theme_label_database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chuangcaleb/Documents/1Notts/fyp/music-theme-recognition/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chuangcaleb/Documents/1Notts/fyp/music-theme-recognition/data/labels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0639EDF-A954-2140-B0B4-DE36733318D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11309809-2FDF-CB4B-AC7B-3E00813B1076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10563,10 +10563,10 @@
   <dimension ref="A1:AC3344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B519" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2951" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="P2974" sqref="P2974"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -47312,6 +47312,9 @@
       <c r="O2972">
         <v>0</v>
       </c>
+      <c r="P2972">
+        <v>0</v>
+      </c>
       <c r="Q2972">
         <v>0</v>
       </c>

</xml_diff>